<commit_message>
Initial commit for urbssolarextension_v1.0
added location to technology params
</commit_message>
<xml_diff>
--- a/Input_urbsextensionv1.xlsx
+++ b/Input_urbsextensionv1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerald\Desktop\urbssolar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxoi\PycharmProjects\urbssolar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605EEEA2-4AFF-4F2E-B423-03CBFFA58F42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2C49998-AA3C-417C-A7CC-91ED7B5AFE38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="5" xr2:uid="{81864710-3A67-40FC-ABA1-4EF02E4F8A12}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="4" xr2:uid="{81864710-3A67-40FC-ABA1-4EF02E4F8A12}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="10" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>Value</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>EU27_solarPV</t>
+  </si>
+  <si>
+    <t>EU27.solarPV</t>
   </si>
 </sst>
 </file>
@@ -641,9 +644,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -651,7 +654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -659,7 +662,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -667,7 +670,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -688,14 +691,14 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" customWidth="1"/>
-    <col min="4" max="4" width="37.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" customWidth="1"/>
+    <col min="4" max="4" width="37.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -709,7 +712,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2024</v>
       </c>
@@ -723,7 +726,7 @@
         <v>414000</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2025</v>
       </c>
@@ -737,7 +740,7 @@
         <v>414000</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2026</v>
       </c>
@@ -751,7 +754,7 @@
         <v>414000</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2027</v>
       </c>
@@ -765,7 +768,7 @@
         <v>414000</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2028</v>
       </c>
@@ -779,7 +782,7 @@
         <v>414000</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2029</v>
       </c>
@@ -793,7 +796,7 @@
         <v>414000</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2030</v>
       </c>
@@ -807,7 +810,7 @@
         <v>414000</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2031</v>
       </c>
@@ -821,7 +824,7 @@
         <v>414000</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2032</v>
       </c>
@@ -835,7 +838,7 @@
         <v>414000</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2033</v>
       </c>
@@ -849,7 +852,7 @@
         <v>414000</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2034</v>
       </c>
@@ -863,7 +866,7 @@
         <v>414000</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2035</v>
       </c>
@@ -877,7 +880,7 @@
         <v>414000</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2036</v>
       </c>
@@ -891,7 +894,7 @@
         <v>414000</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2037</v>
       </c>
@@ -905,7 +908,7 @@
         <v>414000</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2038</v>
       </c>
@@ -919,7 +922,7 @@
         <v>414000</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2039</v>
       </c>
@@ -933,7 +936,7 @@
         <v>414000</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2040</v>
       </c>
@@ -947,7 +950,7 @@
         <v>414000</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2041</v>
       </c>
@@ -961,7 +964,7 @@
         <v>414000</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2042</v>
       </c>
@@ -975,7 +978,7 @@
         <v>414000</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2043</v>
       </c>
@@ -989,7 +992,7 @@
         <v>414000</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2044</v>
       </c>
@@ -1003,7 +1006,7 @@
         <v>414000</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2045</v>
       </c>
@@ -1017,7 +1020,7 @@
         <v>414000</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2046</v>
       </c>
@@ -1031,7 +1034,7 @@
         <v>414000</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2047</v>
       </c>
@@ -1045,7 +1048,7 @@
         <v>414000</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2048</v>
       </c>
@@ -1059,7 +1062,7 @@
         <v>414000</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2049</v>
       </c>
@@ -1073,7 +1076,7 @@
         <v>414000</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2050</v>
       </c>
@@ -1100,64 +1103,64 @@
       <selection activeCell="C1" sqref="C1:H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
     </row>
   </sheetData>
@@ -1173,9 +1176,9 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>20</v>
       </c>
@@ -1183,7 +1186,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <v>0</v>
       </c>
@@ -1191,7 +1194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -1208,23 +1211,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71493739-45C2-4A8D-9266-24BB3FC8F4DB}">
   <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" customWidth="1"/>
-    <col min="10" max="10" width="21.85546875" customWidth="1"/>
-    <col min="14" max="14" width="20.140625" customWidth="1"/>
+    <col min="9" max="9" width="19.33203125" customWidth="1"/>
+    <col min="10" max="10" width="21.88671875" customWidth="1"/>
+    <col min="14" max="14" width="20.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>19</v>
       </c>
@@ -1271,9 +1274,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B2" s="7">
         <v>260000</v>
@@ -1318,52 +1321,52 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
     </row>
   </sheetData>
@@ -1376,13 +1379,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69FD329D-454B-4A8C-B502-49D79ABB4242}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1393,7 +1396,7 @@
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2024</v>
       </c>
@@ -1401,7 +1404,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2025</v>
       </c>
@@ -1409,7 +1412,7 @@
         <v>2.2200000000000001E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2026</v>
       </c>
@@ -1417,7 +1420,7 @@
         <v>2.4400000000000002E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2027</v>
       </c>
@@ -1425,7 +1428,7 @@
         <v>2.6599999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2028</v>
       </c>
@@ -1433,7 +1436,7 @@
         <v>2.8799999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2029</v>
       </c>
@@ -1441,7 +1444,7 @@
         <v>3.1E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2030</v>
       </c>
@@ -1449,7 +1452,7 @@
         <v>3.32E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2031</v>
       </c>
@@ -1457,7 +1460,7 @@
         <v>3.5400000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2032</v>
       </c>
@@ -1465,7 +1468,7 @@
         <v>3.7600000000000001E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2033</v>
       </c>
@@ -1473,7 +1476,7 @@
         <v>3.9800000000000002E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2034</v>
       </c>
@@ -1481,7 +1484,7 @@
         <v>3.9800000000000002E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2035</v>
       </c>
@@ -1489,7 +1492,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2036</v>
       </c>
@@ -1497,7 +1500,7 @@
         <v>4.4200000000000003E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2037</v>
       </c>
@@ -1505,7 +1508,7 @@
         <v>4.6399999999999997E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2038</v>
       </c>
@@ -1513,7 +1516,7 @@
         <v>4.8599999999999997E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2039</v>
       </c>
@@ -1521,7 +1524,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2040</v>
       </c>
@@ -1529,7 +1532,7 @@
         <v>5.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2041</v>
       </c>
@@ -1537,7 +1540,7 @@
         <v>5.5199999999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2042</v>
       </c>
@@ -1545,7 +1548,7 @@
         <v>5.74E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2043</v>
       </c>
@@ -1553,7 +1556,7 @@
         <v>5.96E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2044</v>
       </c>
@@ -1561,7 +1564,7 @@
         <v>6.1800000000000001E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2045</v>
       </c>
@@ -1569,7 +1572,7 @@
         <v>6.4000000000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2046</v>
       </c>
@@ -1577,7 +1580,7 @@
         <v>6.6199999999999995E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2047</v>
       </c>
@@ -1585,7 +1588,7 @@
         <v>6.8400000000000002E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2048</v>
       </c>
@@ -1593,7 +1596,7 @@
         <v>7.0599999999999996E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2049</v>
       </c>
@@ -1601,7 +1604,7 @@
         <v>7.2800000000000004E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2050</v>
       </c>
@@ -1622,9 +1625,9 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1635,7 +1638,7 @@
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2024</v>
       </c>
@@ -1643,7 +1646,7 @@
         <v>26229.707720000002</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2025</v>
       </c>
@@ -1651,7 +1654,7 @@
         <v>26589.174669999997</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2026</v>
       </c>
@@ -1659,7 +1662,7 @@
         <v>60431.69513</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2027</v>
       </c>
@@ -1667,7 +1670,7 @@
         <v>95314.195130000007</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2028</v>
       </c>
@@ -1675,7 +1678,7 @@
         <v>130196.6951</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2029</v>
       </c>
@@ -1683,7 +1686,7 @@
         <v>165780.465</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2030</v>
       </c>
@@ -1691,7 +1694,7 @@
         <v>179750.54879999999</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2031</v>
       </c>
@@ -1699,7 +1702,7 @@
         <v>195610.7611</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2032</v>
       </c>
@@ -1707,7 +1710,7 @@
         <v>196499.72339999999</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2033</v>
       </c>
@@ -1715,7 +1718,7 @@
         <v>198853.9976</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2034</v>
       </c>
@@ -1723,7 +1726,7 @@
         <v>202089.00579999998</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2035</v>
       </c>
@@ -1731,7 +1734,7 @@
         <v>164077.8836</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2036</v>
       </c>
@@ -1739,7 +1742,7 @@
         <v>126654.49769999999</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2037</v>
       </c>
@@ -1747,7 +1750,7 @@
         <v>90701.344779999999</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2038</v>
       </c>
@@ -1755,7 +1758,7 @@
         <v>57298.538379999998</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2039</v>
       </c>
@@ -1763,7 +1766,7 @@
         <v>40938.322699999997</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2040</v>
       </c>
@@ -1771,7 +1774,7 @@
         <v>30788.296410000003</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2041</v>
       </c>
@@ -1779,7 +1782,7 @@
         <v>28368.054080000002</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2042</v>
       </c>
@@ -1787,7 +1790,7 @@
         <v>31250.81408</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2043</v>
       </c>
@@ -1795,7 +1798,7 @@
         <v>34011.350160000002</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2044</v>
       </c>
@@ -1803,7 +1806,7 @@
         <v>35066.675019999995</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2045</v>
       </c>
@@ -1811,7 +1814,7 @@
         <v>33453.543590000001</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2046</v>
       </c>
@@ -1819,7 +1822,7 @@
         <v>25310.301890000002</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2047</v>
       </c>
@@ -1827,7 +1830,7 @@
         <v>11877.08452</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2048</v>
       </c>
@@ -1835,7 +1838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2049</v>
       </c>
@@ -1843,7 +1846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2050</v>
       </c>
@@ -1864,9 +1867,9 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1877,7 +1880,7 @@
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2024</v>
       </c>
@@ -1885,7 +1888,7 @@
         <v>93020</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2025</v>
       </c>
@@ -1893,7 +1896,7 @@
         <v>93020</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2026</v>
       </c>
@@ -1901,7 +1904,7 @@
         <v>93020</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2027</v>
       </c>
@@ -1909,7 +1912,7 @@
         <v>93020</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2028</v>
       </c>
@@ -1917,7 +1920,7 @@
         <v>93020</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2029</v>
       </c>
@@ -1925,7 +1928,7 @@
         <v>93020</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2030</v>
       </c>
@@ -1933,7 +1936,7 @@
         <v>93020</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2031</v>
       </c>
@@ -1941,7 +1944,7 @@
         <v>61911.5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2032</v>
       </c>
@@ -1949,7 +1952,7 @@
         <v>61911.5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2033</v>
       </c>
@@ -1957,7 +1960,7 @@
         <v>61911.5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2034</v>
       </c>
@@ -1965,7 +1968,7 @@
         <v>61911.5</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2035</v>
       </c>
@@ -1973,7 +1976,7 @@
         <v>61911.5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2036</v>
       </c>
@@ -1981,7 +1984,7 @@
         <v>61911.5</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2037</v>
       </c>
@@ -1989,7 +1992,7 @@
         <v>61911.5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2038</v>
       </c>
@@ -1997,7 +2000,7 @@
         <v>61911.5</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2039</v>
       </c>
@@ -2005,7 +2008,7 @@
         <v>61911.5</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2040</v>
       </c>
@@ -2013,7 +2016,7 @@
         <v>61911.5</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2041</v>
       </c>
@@ -2021,7 +2024,7 @@
         <v>57655.199999999997</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2042</v>
       </c>
@@ -2029,7 +2032,7 @@
         <v>57655.199999999997</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2043</v>
       </c>
@@ -2037,7 +2040,7 @@
         <v>57655.199999999997</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2044</v>
       </c>
@@ -2045,7 +2048,7 @@
         <v>57655.199999999997</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2045</v>
       </c>
@@ -2053,7 +2056,7 @@
         <v>57655.199999999997</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2046</v>
       </c>
@@ -2061,7 +2064,7 @@
         <v>57655.199999999997</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2047</v>
       </c>
@@ -2069,7 +2072,7 @@
         <v>57655.199999999997</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2048</v>
       </c>
@@ -2077,7 +2080,7 @@
         <v>57655.199999999997</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2049</v>
       </c>
@@ -2085,7 +2088,7 @@
         <v>57655.199999999997</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2050</v>
       </c>

</xml_diff>

<commit_message>
Edited Output File, report file and exce input
</commit_message>
<xml_diff>
--- a/Input_urbsextensionv1.xlsx
+++ b/Input_urbsextensionv1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxoi\PycharmProjects\urbssolar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2C49998-AA3C-417C-A7CC-91ED7B5AFE38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E7C067-2202-412A-A1CE-F951A5D44F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="4" xr2:uid="{81864710-3A67-40FC-ABA1-4EF02E4F8A12}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{81864710-3A67-40FC-ABA1-4EF02E4F8A12}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="10" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
   <si>
     <t>Value</t>
   </si>
@@ -133,6 +133,21 @@
   </si>
   <si>
     <t>EU27.solarPV</t>
+  </si>
+  <si>
+    <t>import_EU27_windoff</t>
+  </si>
+  <si>
+    <t>manufacturing_EU27_windoff</t>
+  </si>
+  <si>
+    <t>remanufacturing_EU27_windoff</t>
+  </si>
+  <si>
+    <t>EU27.windoff</t>
+  </si>
+  <si>
+    <t>EU27_windoff</t>
   </si>
 </sst>
 </file>
@@ -640,7 +655,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31FF74EF-7037-4139-88AF-F295C305C1F7}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -685,10 +700,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6185AF38-42FD-4CFF-B287-2FCFFF6C6EF3}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="E2" sqref="E2:F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -698,7 +713,7 @@
     <col min="4" max="4" width="37.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -711,8 +726,17 @@
       <c r="D1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2024</v>
       </c>
@@ -725,8 +749,17 @@
       <c r="D2">
         <v>414000</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <v>250240</v>
+      </c>
+      <c r="F2">
+        <v>303600</v>
+      </c>
+      <c r="G2">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2025</v>
       </c>
@@ -739,8 +772,17 @@
       <c r="D3">
         <v>414000</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <v>246486.39999999999</v>
+      </c>
+      <c r="F3">
+        <v>299045.40000000002</v>
+      </c>
+      <c r="G3">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2026</v>
       </c>
@@ -753,8 +795,17 @@
       <c r="D4">
         <v>414000</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>242789.10399999999</v>
+      </c>
+      <c r="F4">
+        <v>294559.71899999998</v>
+      </c>
+      <c r="G4">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2027</v>
       </c>
@@ -767,8 +818,17 @@
       <c r="D5">
         <v>414000</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5">
+        <v>239147.26740000001</v>
+      </c>
+      <c r="F5">
+        <v>290141.32319999998</v>
+      </c>
+      <c r="G5">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2028</v>
       </c>
@@ -781,8 +841,17 @@
       <c r="D6">
         <v>414000</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6">
+        <v>235560.05840000001</v>
+      </c>
+      <c r="F6">
+        <v>285788.2034</v>
+      </c>
+      <c r="G6">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2029</v>
       </c>
@@ -795,8 +864,17 @@
       <c r="D7">
         <v>414000</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <v>232026.65760000001</v>
+      </c>
+      <c r="F7">
+        <v>281498.4804</v>
+      </c>
+      <c r="G7">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2030</v>
       </c>
@@ -809,8 +887,17 @@
       <c r="D8">
         <v>414000</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <v>228546.25769999999</v>
+      </c>
+      <c r="F8">
+        <v>277270.34419999999</v>
+      </c>
+      <c r="G8">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2031</v>
       </c>
@@ -823,8 +910,17 @@
       <c r="D9">
         <v>414000</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9">
+        <v>225118.0638</v>
+      </c>
+      <c r="F9">
+        <v>273102.28909999999</v>
+      </c>
+      <c r="G9">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2032</v>
       </c>
@@ -837,8 +933,17 @@
       <c r="D10">
         <v>414000</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10">
+        <v>221741.2929</v>
+      </c>
+      <c r="F10">
+        <v>268993.2548</v>
+      </c>
+      <c r="G10">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2033</v>
       </c>
@@ -851,8 +956,17 @@
       <c r="D11">
         <v>414000</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E11">
+        <v>218415.1735</v>
+      </c>
+      <c r="F11">
+        <v>264942.41499999998</v>
+      </c>
+      <c r="G11">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2034</v>
       </c>
@@ -865,8 +979,17 @@
       <c r="D12">
         <v>414000</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E12">
+        <v>215138.94589999999</v>
+      </c>
+      <c r="F12">
+        <v>260948.7948</v>
+      </c>
+      <c r="G12">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2035</v>
       </c>
@@ -879,8 +1002,17 @@
       <c r="D13">
         <v>414000</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E13">
+        <v>211911.86170000001</v>
+      </c>
+      <c r="F13">
+        <v>257011.4613</v>
+      </c>
+      <c r="G13">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2036</v>
       </c>
@@ -893,8 +1025,17 @@
       <c r="D14">
         <v>414000</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E14">
+        <v>208733.1838</v>
+      </c>
+      <c r="F14">
+        <v>253129.39139999999</v>
+      </c>
+      <c r="G14">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2037</v>
       </c>
@@ -907,8 +1048,17 @@
       <c r="D15">
         <v>414000</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E15">
+        <v>205602.18599999999</v>
+      </c>
+      <c r="F15">
+        <v>249301.63759999999</v>
+      </c>
+      <c r="G15">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2038</v>
       </c>
@@ -921,8 +1071,17 @@
       <c r="D16">
         <v>414000</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E16">
+        <v>202518.1532</v>
+      </c>
+      <c r="F16">
+        <v>245527.30809999999</v>
+      </c>
+      <c r="G16">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2039</v>
       </c>
@@ -935,8 +1094,17 @@
       <c r="D17">
         <v>414000</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17">
+        <v>199480.38089999999</v>
+      </c>
+      <c r="F17">
+        <v>241805.39859999999</v>
+      </c>
+      <c r="G17">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2040</v>
       </c>
@@ -949,8 +1117,17 @@
       <c r="D18">
         <v>414000</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E18">
+        <v>196488.1752</v>
+      </c>
+      <c r="F18">
+        <v>238134.9901</v>
+      </c>
+      <c r="G18">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2041</v>
       </c>
@@ -963,8 +1140,17 @@
       <c r="D19">
         <v>414000</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E19">
+        <v>193540.85260000001</v>
+      </c>
+      <c r="F19">
+        <v>234515.065</v>
+      </c>
+      <c r="G19">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2042</v>
       </c>
@@ -977,8 +1163,17 @@
       <c r="D20">
         <v>414000</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E20">
+        <v>190637.73980000001</v>
+      </c>
+      <c r="F20">
+        <v>230944.68799999999</v>
+      </c>
+      <c r="G20">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2043</v>
       </c>
@@ -991,8 +1186,17 @@
       <c r="D21">
         <v>414000</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E21">
+        <v>187778.17370000001</v>
+      </c>
+      <c r="F21">
+        <v>227422.96530000001</v>
+      </c>
+      <c r="G21">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2044</v>
       </c>
@@ -1005,8 +1209,17 @@
       <c r="D22">
         <v>414000</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E22">
+        <v>184961.50109999999</v>
+      </c>
+      <c r="F22">
+        <v>223948.88099999999</v>
+      </c>
+      <c r="G22">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2045</v>
       </c>
@@ -1019,8 +1232,17 @@
       <c r="D23">
         <v>414000</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E23">
+        <v>182187.07860000001</v>
+      </c>
+      <c r="F23">
+        <v>220521.46350000001</v>
+      </c>
+      <c r="G23">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2046</v>
       </c>
@@ -1033,8 +1255,17 @@
       <c r="D24">
         <v>414000</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E24">
+        <v>179454.27239999999</v>
+      </c>
+      <c r="F24">
+        <v>217139.74350000001</v>
+      </c>
+      <c r="G24">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2047</v>
       </c>
@@ -1047,8 +1278,17 @@
       <c r="D25">
         <v>414000</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E25">
+        <v>176762.4583</v>
+      </c>
+      <c r="F25">
+        <v>213802.75769999999</v>
+      </c>
+      <c r="G25">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2048</v>
       </c>
@@ -1061,8 +1301,17 @@
       <c r="D26">
         <v>414000</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E26">
+        <v>174111.0214</v>
+      </c>
+      <c r="F26">
+        <v>210509.61679999999</v>
+      </c>
+      <c r="G26">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2049</v>
       </c>
@@ -1075,8 +1324,17 @@
       <c r="D27">
         <v>414000</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E27">
+        <v>171499.3561</v>
+      </c>
+      <c r="F27">
+        <v>207259.3126</v>
+      </c>
+      <c r="G27">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2050</v>
       </c>
@@ -1088,6 +1346,15 @@
       </c>
       <c r="D28">
         <v>414000</v>
+      </c>
+      <c r="E28">
+        <v>168926.8658</v>
+      </c>
+      <c r="F28">
+        <v>204050.9535</v>
+      </c>
+      <c r="G28">
+        <v>600000</v>
       </c>
     </row>
   </sheetData>
@@ -1211,8 +1478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71493739-45C2-4A8D-9266-24BB3FC8F4DB}">
   <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1322,7 +1589,51 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
+      <c r="A3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3">
+        <v>100000</v>
+      </c>
+      <c r="C3">
+        <v>10000</v>
+      </c>
+      <c r="D3">
+        <v>25</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="F3" s="7">
+        <v>0</v>
+      </c>
+      <c r="G3" s="7">
+        <v>1500</v>
+      </c>
+      <c r="H3" s="7">
+        <v>0</v>
+      </c>
+      <c r="I3" s="7">
+        <v>0.37409999999999999</v>
+      </c>
+      <c r="J3" s="7">
+        <v>0.38879999999999998</v>
+      </c>
+      <c r="K3" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="L3" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="M3">
+        <v>25</v>
+      </c>
+      <c r="N3" s="7">
+        <v>5</v>
+      </c>
+      <c r="O3" s="7">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
@@ -1380,7 +1691,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1392,7 +1703,9 @@
       <c r="B1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="5"/>
+      <c r="C1" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
@@ -1403,6 +1716,9 @@
       <c r="B2">
         <v>0.02</v>
       </c>
+      <c r="C2">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -1411,6 +1727,9 @@
       <c r="B3" s="2">
         <v>2.2200000000000001E-2</v>
       </c>
+      <c r="C3" s="2">
+        <v>2.2200000000000001E-2</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
@@ -1419,6 +1738,9 @@
       <c r="B4" s="2">
         <v>2.4400000000000002E-2</v>
       </c>
+      <c r="C4" s="2">
+        <v>2.4400000000000002E-2</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -1427,6 +1749,9 @@
       <c r="B5" s="2">
         <v>2.6599999999999999E-2</v>
       </c>
+      <c r="C5" s="2">
+        <v>2.6599999999999999E-2</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
@@ -1435,6 +1760,9 @@
       <c r="B6" s="2">
         <v>2.8799999999999999E-2</v>
       </c>
+      <c r="C6" s="2">
+        <v>2.8799999999999999E-2</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
@@ -1443,6 +1771,9 @@
       <c r="B7" s="2">
         <v>3.1E-2</v>
       </c>
+      <c r="C7" s="2">
+        <v>3.1E-2</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -1451,6 +1782,9 @@
       <c r="B8" s="2">
         <v>3.32E-2</v>
       </c>
+      <c r="C8" s="2">
+        <v>3.32E-2</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
@@ -1459,6 +1793,9 @@
       <c r="B9" s="2">
         <v>3.5400000000000001E-2</v>
       </c>
+      <c r="C9" s="2">
+        <v>3.5400000000000001E-2</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -1467,6 +1804,9 @@
       <c r="B10" s="2">
         <v>3.7600000000000001E-2</v>
       </c>
+      <c r="C10" s="2">
+        <v>3.7600000000000001E-2</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
@@ -1475,6 +1815,9 @@
       <c r="B11" s="2">
         <v>3.9800000000000002E-2</v>
       </c>
+      <c r="C11" s="2">
+        <v>3.9800000000000002E-2</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
@@ -1483,6 +1826,9 @@
       <c r="B12" s="2">
         <v>3.9800000000000002E-2</v>
       </c>
+      <c r="C12" s="2">
+        <v>3.9800000000000002E-2</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
@@ -1491,6 +1837,9 @@
       <c r="B13" s="2">
         <v>4.2000000000000003E-2</v>
       </c>
+      <c r="C13" s="2">
+        <v>4.2000000000000003E-2</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
@@ -1499,6 +1848,9 @@
       <c r="B14" s="2">
         <v>4.4200000000000003E-2</v>
       </c>
+      <c r="C14" s="2">
+        <v>4.4200000000000003E-2</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
@@ -1507,6 +1859,9 @@
       <c r="B15" s="2">
         <v>4.6399999999999997E-2</v>
       </c>
+      <c r="C15" s="2">
+        <v>4.6399999999999997E-2</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
@@ -1515,100 +1870,139 @@
       <c r="B16" s="2">
         <v>4.8599999999999997E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C16" s="2">
+        <v>4.8599999999999997E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2039</v>
       </c>
       <c r="B17" s="2">
         <v>5.0799999999999998E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C17" s="2">
+        <v>5.0799999999999998E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2040</v>
       </c>
       <c r="B18" s="2">
         <v>5.2999999999999999E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C18" s="2">
+        <v>5.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2041</v>
       </c>
       <c r="B19" s="2">
         <v>5.5199999999999999E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C19" s="2">
+        <v>5.5199999999999999E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2042</v>
       </c>
       <c r="B20" s="2">
         <v>5.74E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C20" s="2">
+        <v>5.74E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2043</v>
       </c>
       <c r="B21" s="2">
         <v>5.96E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C21" s="2">
+        <v>5.96E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2044</v>
       </c>
       <c r="B22" s="2">
         <v>6.1800000000000001E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C22" s="2">
+        <v>6.1800000000000001E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2045</v>
       </c>
       <c r="B23" s="2">
         <v>6.4000000000000001E-2</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C23" s="2">
+        <v>6.4000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2046</v>
       </c>
       <c r="B24" s="2">
         <v>6.6199999999999995E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C24" s="2">
+        <v>6.6199999999999995E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2047</v>
       </c>
       <c r="B25" s="2">
         <v>6.8400000000000002E-2</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C25" s="2">
+        <v>6.8400000000000002E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2048</v>
       </c>
       <c r="B26" s="2">
         <v>7.0599999999999996E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C26" s="2">
+        <v>7.0599999999999996E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2049</v>
       </c>
       <c r="B27" s="2">
         <v>7.2800000000000004E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C27" s="2">
+        <v>7.2800000000000004E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2050</v>
       </c>
       <c r="B28">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="C28">
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
@@ -1622,7 +2016,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1634,7 +2028,9 @@
       <c r="B1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="5"/>
+      <c r="C1" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
@@ -1645,6 +2041,9 @@
       <c r="B2">
         <v>26229.707720000002</v>
       </c>
+      <c r="C2">
+        <v>26229.707720000002</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -1653,6 +2052,9 @@
       <c r="B3">
         <v>26589.174669999997</v>
       </c>
+      <c r="C3">
+        <v>26589.174669999997</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
@@ -1661,6 +2063,9 @@
       <c r="B4">
         <v>60431.69513</v>
       </c>
+      <c r="C4">
+        <v>60431.69513</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -1669,6 +2074,9 @@
       <c r="B5">
         <v>95314.195130000007</v>
       </c>
+      <c r="C5">
+        <v>95314.195130000007</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
@@ -1677,6 +2085,9 @@
       <c r="B6">
         <v>130196.6951</v>
       </c>
+      <c r="C6">
+        <v>130196.6951</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
@@ -1685,6 +2096,9 @@
       <c r="B7">
         <v>165780.465</v>
       </c>
+      <c r="C7">
+        <v>165780.465</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -1693,6 +2107,9 @@
       <c r="B8">
         <v>179750.54879999999</v>
       </c>
+      <c r="C8">
+        <v>179750.54879999999</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
@@ -1701,6 +2118,9 @@
       <c r="B9">
         <v>195610.7611</v>
       </c>
+      <c r="C9">
+        <v>195610.7611</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -1709,6 +2129,9 @@
       <c r="B10">
         <v>196499.72339999999</v>
       </c>
+      <c r="C10">
+        <v>196499.72339999999</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
@@ -1717,6 +2140,9 @@
       <c r="B11">
         <v>198853.9976</v>
       </c>
+      <c r="C11">
+        <v>198853.9976</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
@@ -1725,6 +2151,9 @@
       <c r="B12">
         <v>202089.00579999998</v>
       </c>
+      <c r="C12">
+        <v>202089.00579999998</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
@@ -1733,6 +2162,9 @@
       <c r="B13">
         <v>164077.8836</v>
       </c>
+      <c r="C13">
+        <v>164077.8836</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
@@ -1741,6 +2173,9 @@
       <c r="B14">
         <v>126654.49769999999</v>
       </c>
+      <c r="C14">
+        <v>126654.49769999999</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
@@ -1749,6 +2184,9 @@
       <c r="B15">
         <v>90701.344779999999</v>
       </c>
+      <c r="C15">
+        <v>90701.344779999999</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
@@ -1757,100 +2195,139 @@
       <c r="B16">
         <v>57298.538379999998</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C16">
+        <v>57298.538379999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2039</v>
       </c>
       <c r="B17">
         <v>40938.322699999997</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C17">
+        <v>40938.322699999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2040</v>
       </c>
       <c r="B18">
         <v>30788.296410000003</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <v>30788.296410000003</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2041</v>
       </c>
       <c r="B19">
         <v>28368.054080000002</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C19">
+        <v>28368.054080000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2042</v>
       </c>
       <c r="B20">
         <v>31250.81408</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C20">
+        <v>31250.81408</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2043</v>
       </c>
       <c r="B21">
         <v>34011.350160000002</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C21">
+        <v>34011.350160000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2044</v>
       </c>
       <c r="B22">
         <v>35066.675019999995</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C22">
+        <v>35066.675019999995</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2045</v>
       </c>
       <c r="B23">
         <v>33453.543590000001</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C23">
+        <v>33453.543590000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2046</v>
       </c>
       <c r="B24">
         <v>25310.301890000002</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C24">
+        <v>25310.301890000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2047</v>
       </c>
       <c r="B25">
         <v>11877.08452</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C25">
+        <v>11877.08452</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2048</v>
       </c>
       <c r="B26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2049</v>
       </c>
       <c r="B27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2050</v>
       </c>
       <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
         <v>0</v>
       </c>
     </row>
@@ -1863,8 +2340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3790A601-26C3-4DCA-97B6-9342C547A4A0}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1876,7 +2353,9 @@
       <c r="B1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="5"/>
+      <c r="C1" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
@@ -1887,6 +2366,9 @@
       <c r="B2" s="4">
         <v>93020</v>
       </c>
+      <c r="C2" s="4">
+        <v>30000</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -1895,6 +2377,9 @@
       <c r="B3" s="4">
         <v>93020</v>
       </c>
+      <c r="C3" s="4">
+        <v>30000</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
@@ -1903,6 +2388,9 @@
       <c r="B4" s="4">
         <v>93020</v>
       </c>
+      <c r="C4" s="4">
+        <v>30000</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -1911,6 +2399,9 @@
       <c r="B5" s="4">
         <v>93020</v>
       </c>
+      <c r="C5" s="4">
+        <v>30000</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
@@ -1919,6 +2410,9 @@
       <c r="B6" s="4">
         <v>93020</v>
       </c>
+      <c r="C6" s="4">
+        <v>30000</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
@@ -1927,6 +2421,9 @@
       <c r="B7" s="4">
         <v>93020</v>
       </c>
+      <c r="C7" s="4">
+        <v>30000</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -1935,6 +2432,9 @@
       <c r="B8" s="4">
         <v>93020</v>
       </c>
+      <c r="C8" s="4">
+        <v>30000</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
@@ -1943,6 +2443,9 @@
       <c r="B9" s="4">
         <v>61911.5</v>
       </c>
+      <c r="C9" s="4">
+        <v>30000</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -1951,6 +2454,9 @@
       <c r="B10" s="4">
         <v>61911.5</v>
       </c>
+      <c r="C10" s="4">
+        <v>30000</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
@@ -1959,6 +2465,9 @@
       <c r="B11" s="4">
         <v>61911.5</v>
       </c>
+      <c r="C11" s="4">
+        <v>30000</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
@@ -1967,6 +2476,9 @@
       <c r="B12" s="4">
         <v>61911.5</v>
       </c>
+      <c r="C12" s="4">
+        <v>30000</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
@@ -1975,6 +2487,9 @@
       <c r="B13" s="4">
         <v>61911.5</v>
       </c>
+      <c r="C13" s="4">
+        <v>30000</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
@@ -1983,6 +2498,9 @@
       <c r="B14" s="4">
         <v>61911.5</v>
       </c>
+      <c r="C14" s="4">
+        <v>30000</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
@@ -1991,6 +2509,9 @@
       <c r="B15" s="4">
         <v>61911.5</v>
       </c>
+      <c r="C15" s="4">
+        <v>30000</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
@@ -1999,101 +2520,140 @@
       <c r="B16" s="4">
         <v>61911.5</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C16" s="4">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2039</v>
       </c>
       <c r="B17" s="4">
         <v>61911.5</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C17" s="4">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2040</v>
       </c>
       <c r="B18" s="4">
         <v>61911.5</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C18" s="4">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2041</v>
       </c>
       <c r="B19" s="4">
         <v>57655.199999999997</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C19" s="4">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2042</v>
       </c>
       <c r="B20" s="4">
         <v>57655.199999999997</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C20" s="4">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2043</v>
       </c>
       <c r="B21" s="4">
         <v>57655.199999999997</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C21" s="4">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2044</v>
       </c>
       <c r="B22" s="3">
         <v>57655.199999999997</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C22" s="4">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2045</v>
       </c>
       <c r="B23" s="3">
         <v>57655.199999999997</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C23" s="4">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2046</v>
       </c>
       <c r="B24" s="3">
         <v>57655.199999999997</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C24" s="4">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2047</v>
       </c>
       <c r="B25" s="3">
         <v>57655.199999999997</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C25" s="4">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2048</v>
       </c>
       <c r="B26" s="3">
         <v>57655.199999999997</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C26" s="4">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2049</v>
       </c>
       <c r="B27" s="3">
         <v>57655.199999999997</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C27" s="4">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2050</v>
       </c>
       <c r="B28" s="3">
         <v>57655.199999999997</v>
+      </c>
+      <c r="C28" s="4">
+        <v>30000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Did some testing and cleaned up the code
</commit_message>
<xml_diff>
--- a/Input_urbsextensionv1.xlsx
+++ b/Input_urbsextensionv1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxoi\PycharmProjects\urbssolar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E7C067-2202-412A-A1CE-F951A5D44F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25CF9EF1-ED4E-481B-BA7A-CBC2C7FE66F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{81864710-3A67-40FC-ABA1-4EF02E4F8A12}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{81864710-3A67-40FC-ABA1-4EF02E4F8A12}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="10" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
   <si>
     <t>Value</t>
   </si>
@@ -96,16 +96,10 @@
     <t>EU27</t>
   </si>
   <si>
-    <t>solarPV</t>
-  </si>
-  <si>
     <t>Locations:</t>
   </si>
   <si>
     <t>Technologies</t>
-  </si>
-  <si>
-    <t>timestep</t>
   </si>
   <si>
     <t>InitialStockpile</t>
@@ -655,7 +649,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31FF74EF-7037-4139-88AF-F295C305C1F7}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -718,22 +712,22 @@
         <v>15</v>
       </c>
       <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
         <v>23</v>
       </c>
-      <c r="C1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" t="s">
-        <v>25</v>
-      </c>
       <c r="E1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
         <v>30</v>
-      </c>
-      <c r="F1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -1377,7 +1371,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
@@ -1437,36 +1431,320 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6341E4C-4AB4-44A4-8119-B6BB3BEB6E84}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="7">
-        <v>0</v>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2024</v>
       </c>
       <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="7">
-        <v>1</v>
+        <v>0.125</v>
+      </c>
+      <c r="C2">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2025</v>
       </c>
       <c r="B3">
         <v>0.125</v>
+      </c>
+      <c r="C3">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2026</v>
+      </c>
+      <c r="B4">
+        <v>0.125</v>
+      </c>
+      <c r="C4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2027</v>
+      </c>
+      <c r="B5">
+        <v>0.125</v>
+      </c>
+      <c r="C5">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2028</v>
+      </c>
+      <c r="B6">
+        <v>0.125</v>
+      </c>
+      <c r="C6">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2029</v>
+      </c>
+      <c r="B7">
+        <v>0.125</v>
+      </c>
+      <c r="C7">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>2030</v>
+      </c>
+      <c r="B8">
+        <v>0.125</v>
+      </c>
+      <c r="C8">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>2031</v>
+      </c>
+      <c r="B9">
+        <v>0.125</v>
+      </c>
+      <c r="C9">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>2032</v>
+      </c>
+      <c r="B10">
+        <v>0.125</v>
+      </c>
+      <c r="C10">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>2033</v>
+      </c>
+      <c r="B11">
+        <v>0.125</v>
+      </c>
+      <c r="C11">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>2034</v>
+      </c>
+      <c r="B12">
+        <v>0.125</v>
+      </c>
+      <c r="C12">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>2035</v>
+      </c>
+      <c r="B13">
+        <v>0.125</v>
+      </c>
+      <c r="C13">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>2036</v>
+      </c>
+      <c r="B14">
+        <v>0.125</v>
+      </c>
+      <c r="C14">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>2037</v>
+      </c>
+      <c r="B15">
+        <v>0.125</v>
+      </c>
+      <c r="C15">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>2038</v>
+      </c>
+      <c r="B16">
+        <v>0.125</v>
+      </c>
+      <c r="C16">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>2039</v>
+      </c>
+      <c r="B17">
+        <v>0.125</v>
+      </c>
+      <c r="C17">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>2040</v>
+      </c>
+      <c r="B18">
+        <v>0.125</v>
+      </c>
+      <c r="C18">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>2041</v>
+      </c>
+      <c r="B19">
+        <v>0.125</v>
+      </c>
+      <c r="C19">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>2042</v>
+      </c>
+      <c r="B20">
+        <v>0.125</v>
+      </c>
+      <c r="C20">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>2043</v>
+      </c>
+      <c r="B21">
+        <v>0.125</v>
+      </c>
+      <c r="C21">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>2044</v>
+      </c>
+      <c r="B22">
+        <v>0.125</v>
+      </c>
+      <c r="C22">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>2045</v>
+      </c>
+      <c r="B23">
+        <v>0.125</v>
+      </c>
+      <c r="C23">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>2046</v>
+      </c>
+      <c r="B24">
+        <v>0.125</v>
+      </c>
+      <c r="C24">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>2047</v>
+      </c>
+      <c r="B25">
+        <v>0.125</v>
+      </c>
+      <c r="C25">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>2048</v>
+      </c>
+      <c r="B26">
+        <v>0.125</v>
+      </c>
+      <c r="C26">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>2049</v>
+      </c>
+      <c r="B27">
+        <v>0.125</v>
+      </c>
+      <c r="C27">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>2050</v>
+      </c>
+      <c r="B28">
+        <v>0.125</v>
+      </c>
+      <c r="C28">
+        <v>0.25</v>
       </c>
     </row>
   </sheetData>
@@ -1496,16 +1774,16 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>5</v>
@@ -1529,7 +1807,7 @@
         <v>11</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="M1" s="6" t="s">
         <v>13</v>
@@ -1538,12 +1816,12 @@
         <v>2</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B2" s="7">
         <v>260000</v>
@@ -1590,7 +1868,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B3">
         <v>100000</v>
@@ -1691,7 +1969,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1701,10 +1979,10 @@
         <v>15</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
@@ -2026,10 +2304,10 @@
         <v>15</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
@@ -2351,10 +2629,10 @@
         <v>15</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>

</xml_diff>